<commit_message>
Add SideAva for skill
</commit_message>
<xml_diff>
--- a/LarpCreater/LARP New FrameWork/Assets/Excel/Skill.xlsx
+++ b/LarpCreater/LARP New FrameWork/Assets/Excel/Skill.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LARP Project\LARP_System\LarpCreater\LARP New FrameWork\Assets\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942679DC-67A0-4B06-B1CC-44D0D10BE771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,18 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="125">
-  <si>
-    <t xml:space="preserve">招式名字</t>
-  </si>
-  <si>
-    <t xml:space="preserve">招式圖片</t>
-  </si>
-  <si>
-    <t xml:space="preserve">功能說明</t>
-  </si>
-  <si>
-    <t xml:space="preserve">詳細功能說明</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="127">
+  <si>
+    <t>招式名字</t>
+  </si>
+  <si>
+    <t>招式圖片</t>
+  </si>
+  <si>
+    <t>功能說明</t>
+  </si>
+  <si>
+    <t>詳細功能說明</t>
   </si>
   <si>
     <r>
@@ -42,7 +47,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">可用職業</t>
+      <t>可用職業</t>
     </r>
     <r>
       <rPr>
@@ -52,11 +57,11 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">(W/A/M/V)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">前置技</t>
+      <t>(W/A/M/V)</t>
+    </r>
+  </si>
+  <si>
+    <t>前置技</t>
   </si>
   <si>
     <r>
@@ -67,7 +72,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">增益</t>
+      <t>增益</t>
     </r>
     <r>
       <rPr>
@@ -89,7 +94,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">增益</t>
+      <t>增益</t>
     </r>
     <r>
       <rPr>
@@ -111,7 +116,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">增益</t>
+      <t>增益</t>
     </r>
     <r>
       <rPr>
@@ -133,7 +138,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">增益</t>
+      <t>增益</t>
     </r>
     <r>
       <rPr>
@@ -155,7 +160,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">可用等級</t>
+      <t>可用等級</t>
     </r>
     <r>
       <rPr>
@@ -169,16 +174,16 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">系列最大點數</t>
-  </si>
-  <si>
-    <t xml:space="preserve">急救</t>
-  </si>
-  <si>
-    <t xml:space="preserve">治療術</t>
-  </si>
-  <si>
-    <t xml:space="preserve">治療友方單位</t>
+    <t>系列最大點數</t>
+  </si>
+  <si>
+    <t>急救</t>
+  </si>
+  <si>
+    <t>治療術</t>
+  </si>
+  <si>
+    <t>治療友方單位</t>
   </si>
   <si>
     <r>
@@ -189,7 +194,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">以繃帶治療目標回復2點生命，最多攜帶3條繃帶，無法治療自己。
+      <t>以繃帶治療目標回復2點生命，最多攜帶3條繃帶，無法治療自己。
 也可對臨死目標施予救援。
 同時可重置目標治療以外的使用掉的1個技能。
 施放方式:
@@ -205,68 +210,68 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">在復活點有大於3條繃帶時，治療師可消耗1枚金幣補充3條繃帶。</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">W/A/M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">斬殺</t>
-  </si>
-  <si>
-    <t xml:space="preserve">尾刀回血</t>
-  </si>
-  <si>
-    <t xml:space="preserve">處決目標回血</t>
-  </si>
-  <si>
-    <t xml:space="preserve">處決目標可回復1點生命。
+      <t>在復活點有大於3條繃帶時，治療師可消耗1枚金幣補充3條繃帶。</t>
+    </r>
+  </si>
+  <si>
+    <t>W/A/M</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>斬殺</t>
+  </si>
+  <si>
+    <t>尾刀回血</t>
+  </si>
+  <si>
+    <t>處決目標回血</t>
+  </si>
+  <si>
+    <t>處決目標可回復1點生命。
 施放方式:
 對已經被擊敗的目標演出處決，可回復1點生命。</t>
   </si>
   <si>
-    <t xml:space="preserve">W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">背襲</t>
-  </si>
-  <si>
-    <t xml:space="preserve">背襲回血</t>
-  </si>
-  <si>
-    <t xml:space="preserve">擊中背部回血</t>
-  </si>
-  <si>
-    <t xml:space="preserve">擊中背部回1HP，每個目標只能1次。
+    <t>W</t>
+  </si>
+  <si>
+    <t>背襲</t>
+  </si>
+  <si>
+    <t>背襲回血</t>
+  </si>
+  <si>
+    <t>擊中背部回血</t>
+  </si>
+  <si>
+    <t>擊中背部回1HP，每個目標只能1次。
 說明:
 同個目標1分鐘內只能作用1次。</t>
   </si>
   <si>
-    <t xml:space="preserve">W/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">優勢武裝</t>
-  </si>
-  <si>
-    <t xml:space="preserve">解銷大型武裝</t>
-  </si>
-  <si>
-    <t xml:space="preserve">解鎖140cm以上大型武器
+    <t>W/A</t>
+  </si>
+  <si>
+    <t>優勢武裝</t>
+  </si>
+  <si>
+    <t>解銷大型武裝</t>
+  </si>
+  <si>
+    <t>解鎖140cm以上大型武器
 解鎖80cm以上大型盾牌
 解鎖單手持139以下雙手武器。</t>
   </si>
   <si>
-    <t xml:space="preserve">耐力</t>
-  </si>
-  <si>
-    <t xml:space="preserve">提高生命上限</t>
-  </si>
-  <si>
-    <t xml:space="preserve">生命上限提高1點。</t>
+    <t>耐力</t>
+  </si>
+  <si>
+    <t>提高生命上限</t>
+  </si>
+  <si>
+    <t>生命上限提高1點。</t>
   </si>
   <si>
     <r>
@@ -277,7 +282,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">+</t>
+      <t>+</t>
     </r>
     <r>
       <rPr>
@@ -287,14 +292,14 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">投持武器</t>
-  </si>
-  <si>
-    <t xml:space="preserve">解鎖投持武器</t>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>投持武器</t>
+  </si>
+  <si>
+    <t>解鎖投持武器</t>
   </si>
   <si>
     <r>
@@ -305,7 +310,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">可攜3支投持武器/或</t>
+      <t>可攜3支投持武器/或</t>
     </r>
     <r>
       <rPr>
@@ -315,7 +320,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">NERF MAGA彈</t>
+      <t>NERF MAGA彈</t>
     </r>
     <r>
       <rPr>
@@ -325,7 +330,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">/或</t>
+      <t>/或</t>
     </r>
     <r>
       <rPr>
@@ -335,7 +340,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">NERF</t>
+      <t>NERF</t>
     </r>
     <r>
       <rPr>
@@ -345,19 +350,19 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">弩矢
+      <t>弩矢
 施放方式:
 將中程武器彈射出，造成1點遠程傷害。</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">蓄力打擊</t>
-  </si>
-  <si>
-    <t xml:space="preserve">強力近戰技能</t>
-  </si>
-  <si>
-    <t xml:space="preserve">高舉武器喊出招式後揮擊，造成3點進戰技能傷害。
+    <t>蓄力打擊</t>
+  </si>
+  <si>
+    <t>強力近戰技能</t>
+  </si>
+  <si>
+    <t>高舉武器喊出招式後揮擊，造成3點進戰技能傷害。
 施放方式:
 將武器舉起蓄力並喊出招式名稱，至少2秒2音節。
 帶嚇聲揮擊，可跨出一步。
@@ -366,16 +371,16 @@
 受到急救、群體治療、自我回復、或使用沙漏，可回復技能。</t>
   </si>
   <si>
-    <t xml:space="preserve">大型箭袋</t>
-  </si>
-  <si>
-    <t xml:space="preserve">提高箭矢上限</t>
-  </si>
-  <si>
-    <t xml:space="preserve">箭矢攜帶數量+10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
+    <t>大型箭袋</t>
+  </si>
+  <si>
+    <t>提高箭矢上限</t>
+  </si>
+  <si>
+    <t>箭矢攜帶數量+10</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
   <si>
     <r>
@@ -386,7 +391,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">+</t>
+      <t>+</t>
     </r>
     <r>
       <rPr>
@@ -396,17 +401,17 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">10</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">火箭</t>
-  </si>
-  <si>
-    <t xml:space="preserve">火焰箭</t>
-  </si>
-  <si>
-    <t xml:space="preserve">強力遠程技能</t>
+      <t>10</t>
+    </r>
+  </si>
+  <si>
+    <t>火箭</t>
+  </si>
+  <si>
+    <t>火焰箭</t>
+  </si>
+  <si>
+    <t>強力遠程技能</t>
   </si>
   <si>
     <t xml:space="preserve">可攜帶1支可造成3法傷的火焰箭矢
@@ -418,13 +423,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">多重箭</t>
-  </si>
-  <si>
-    <t xml:space="preserve">解鎖多重箭</t>
-  </si>
-  <si>
-    <t xml:space="preserve">可一次射出多隻箭矢。
+    <t>多重箭</t>
+  </si>
+  <si>
+    <t>解鎖多重箭</t>
+  </si>
+  <si>
+    <t>可一次射出多隻箭矢。
 被動:+3箭矢
 施放方式:
 架好2~3支箭矢一次射出(建議橫拿弓)
@@ -439,7 +444,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">+</t>
+      <t>+</t>
     </r>
     <r>
       <rPr>
@@ -449,14 +454,14 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">3</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">恐懼術</t>
-  </si>
-  <si>
-    <t xml:space="preserve">使目標逃跑</t>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <t>恐懼術</t>
+  </si>
+  <si>
+    <t>使目標逃跑</t>
   </si>
   <si>
     <r>
@@ -481,20 +486,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">受到急救、群體治療、自我回復、或使用沙漏，可回復技能。</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">冰凍</t>
-  </si>
-  <si>
-    <t xml:space="preserve">冰凍術</t>
-  </si>
-  <si>
-    <t xml:space="preserve">定身爆擊目標</t>
+      <t>受到急救、群體治療、自我回復、或使用沙漏，可回復技能。</t>
+    </r>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>冰凍</t>
+  </si>
+  <si>
+    <t>冰凍術</t>
+  </si>
+  <si>
+    <t>定身爆擊目標</t>
   </si>
   <si>
     <r>
@@ -517,7 +522,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">施放方式:
+      <t>施放方式:
 於三步範圍內，讀出帶有冰系關鍵字的技能名稱。
 手指目標的腳喊"冰凍"，造成目標雙腳不能移動持續5秒，
 受到任何傷害將會解除定身，並造成額外1點傷害。
@@ -525,13 +530,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">加速法陣</t>
-  </si>
-  <si>
-    <t xml:space="preserve">法陣部署</t>
-  </si>
-  <si>
-    <t xml:space="preserve">學會加速法陣</t>
+    <t>加速法陣</t>
+  </si>
+  <si>
+    <t>法陣部署</t>
+  </si>
+  <si>
+    <t>學會加速法陣</t>
   </si>
   <si>
     <r>
@@ -561,33 +566,33 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">被動:法力上限提高1點</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">魔法衛士</t>
-  </si>
-  <si>
-    <t xml:space="preserve">戰鬥法師</t>
-  </si>
-  <si>
-    <t xml:space="preserve">獲得中型盾牌</t>
-  </si>
-  <si>
-    <t xml:space="preserve">解鎖中型盾牌，但法球減少3顆。</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">魔力充沛</t>
+      <t>被動:法力上限提高1點</t>
+    </r>
+  </si>
+  <si>
+    <t>魔法衛士</t>
+  </si>
+  <si>
+    <t>戰鬥法師</t>
+  </si>
+  <si>
+    <t>獲得中型盾牌</t>
+  </si>
+  <si>
+    <t>解鎖中型盾牌，但法球減少3顆。</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>魔力充沛</t>
   </si>
   <si>
     <t xml:space="preserve">
 提高法力上限</t>
   </si>
   <si>
-    <t xml:space="preserve">法球攜帶量加倍，
+    <t>法球攜帶量加倍，
 但生命降低1點。</t>
   </si>
   <si>
@@ -599,7 +604,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">-</t>
+      <t>-</t>
     </r>
     <r>
       <rPr>
@@ -609,17 +614,17 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">x2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">祝福</t>
-  </si>
-  <si>
-    <t xml:space="preserve">強化友方生命</t>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>祝福</t>
+  </si>
+  <si>
+    <t>強化友方生命</t>
   </si>
   <si>
     <r>
@@ -644,20 +649,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">被動:淨化-以法器觸碰友方能解除控制效果。</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">大師耐力</t>
-  </si>
-  <si>
-    <t xml:space="preserve">生命上限提高3點。</t>
-  </si>
-  <si>
-    <t xml:space="preserve">強化耐力</t>
-  </si>
-  <si>
-    <t xml:space="preserve">生命上限提高2點。</t>
+      <t>被動:淨化-以法器觸碰友方能解除控制效果。</t>
+    </r>
+  </si>
+  <si>
+    <t>大師耐力</t>
+  </si>
+  <si>
+    <t>生命上限提高3點。</t>
+  </si>
+  <si>
+    <t>強化耐力</t>
+  </si>
+  <si>
+    <t>生命上限提高2點。</t>
   </si>
   <si>
     <r>
@@ -668,7 +673,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">+</t>
+      <t>+</t>
     </r>
     <r>
       <rPr>
@@ -678,22 +683,22 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">2</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">投持大師</t>
-  </si>
-  <si>
-    <t xml:space="preserve">提高投持數量</t>
-  </si>
-  <si>
-    <t xml:space="preserve">可攜6支投持武器/或NERF MAGA彈/或NERF弩矢
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>投持大師</t>
+  </si>
+  <si>
+    <t>提高投持數量</t>
+  </si>
+  <si>
+    <t>可攜6支投持武器/或NERF MAGA彈/或NERF弩矢
 施放方式:
 將中程武器彈射出，造成1點遠程傷害。</t>
   </si>
   <si>
-    <t xml:space="preserve">火箭大師</t>
+    <t>火箭大師</t>
   </si>
   <si>
     <r>
@@ -715,7 +720,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">施放方式:
+      <t>施放方式:
 以代表火焰的紅色布套，建議加裝鈴鐺，安裝於箭矢上。
 射擊時需喊出與火有關的射擊技能名稱(例如:火焰箭!)
 擊中目標造成3點技能傷害，無視格檔。
@@ -723,10 +728,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">群體治療</t>
-  </si>
-  <si>
-    <t xml:space="preserve">治療複數單位</t>
+    <t>群體治療</t>
+  </si>
+  <si>
+    <t>治療複數單位</t>
   </si>
   <si>
     <r>
@@ -758,7 +763,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">施放方式:
+      <t>施放方式:
 舉起代表治療的道具或武器，呼喚友方來觸碰。
 如果集結人數超過3人，喊滿!
 帶所需治療目標都碰到時，喊出代表治療的技能名稱。
@@ -769,13 +774,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">戰鬥武裝</t>
-  </si>
-  <si>
-    <t xml:space="preserve">學會戰鬥武裝</t>
-  </si>
-  <si>
-    <t xml:space="preserve">解鎖硬甲、雙手武器，並能用法杖作戰。
+    <t>戰鬥武裝</t>
+  </si>
+  <si>
+    <t>學會戰鬥武裝</t>
+  </si>
+  <si>
+    <t>解鎖硬甲、雙手武器，並能用法杖作戰。
 但法力減少2點。
 法杖:長度不限，但需安全檢驗合格。
 法杖只有擊中軀幹才會造成傷害。
@@ -783,10 +788,10 @@
 硬甲:肩、手、小腿的硬質盔甲能抵擋1點近戰攻擊。</t>
   </si>
   <si>
-    <t xml:space="preserve">震地擊</t>
-  </si>
-  <si>
-    <t xml:space="preserve">範圍震暈敵人</t>
+    <t>震地擊</t>
+  </si>
+  <si>
+    <t>範圍震暈敵人</t>
   </si>
   <si>
     <r>
@@ -814,21 +819,21 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">受到急救、群體治療、自我回復、或使用沙漏，可回復技能。</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">鏡面盾牌</t>
-  </si>
-  <si>
-    <t xml:space="preserve">降低魔法傷害</t>
+      <t>受到急救、群體治療、自我回復、或使用沙漏，可回復技能。</t>
+    </r>
+  </si>
+  <si>
+    <t>鏡面盾牌</t>
+  </si>
+  <si>
+    <t>降低魔法傷害</t>
   </si>
   <si>
     <t xml:space="preserve">
 使盾牌能抵擋1點法傷</t>
   </si>
   <si>
-    <t xml:space="preserve">擊退</t>
+    <t>擊退</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -863,26 +868,26 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">自我恢復</t>
-  </si>
-  <si>
-    <t xml:space="preserve">對自己治療</t>
-  </si>
-  <si>
-    <t xml:space="preserve">消耗補給治療自己4點生命，並回復1個技能，無法治療他人。
+    <t>自我恢復</t>
+  </si>
+  <si>
+    <t>對自己治療</t>
+  </si>
+  <si>
+    <t>消耗補給治療自己4點生命，並回復1個技能，無法治療他人。
 施放方式:
 於復活點消耗1枚金幣，使用治療藥水、飲食、或其他合理道具。
 同時可重置治療以外的使用掉的1個技能。
 (第一次使用就需消耗)</t>
   </si>
   <si>
-    <t xml:space="preserve">潛行</t>
-  </si>
-  <si>
-    <t xml:space="preserve">挑選進場位置</t>
-  </si>
-  <si>
-    <t xml:space="preserve">潛行於場邊繞行，於有利時機進場。
+    <t>潛行</t>
+  </si>
+  <si>
+    <t>挑選進場位置</t>
+  </si>
+  <si>
+    <t>潛行於場邊繞行，於有利時機進場。
 施放方式:
 使用樹葉隱匿身體後進入潛行，將視為不可見目標，無法被攻擊。
 持樹葉時可於場邊繞行，拋棄樹葉後即進場。
@@ -890,10 +895,10 @@
 陣亡後可以靈魂狀態撿回樹葉、或由其他場務人員拾回，下條命可再度使用。</t>
   </si>
   <si>
-    <t xml:space="preserve">防禦法陣</t>
-  </si>
-  <si>
-    <t xml:space="preserve">抵擋遠程攻擊</t>
+    <t>防禦法陣</t>
+  </si>
+  <si>
+    <t>抵擋遠程攻擊</t>
   </si>
   <si>
     <t xml:space="preserve">將法帶排成一線，持續引導製造魔法壁障，抵擋遠程與魔傷害。
@@ -909,21 +914,21 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">複合護甲</t>
-  </si>
-  <si>
-    <t xml:space="preserve">高級物理防禦</t>
-  </si>
-  <si>
-    <t xml:space="preserve">同時獲得硬甲與韌甲
+    <t>複合護甲</t>
+  </si>
+  <si>
+    <t>高級物理防禦</t>
+  </si>
+  <si>
+    <t>同時獲得硬甲與韌甲
 硬甲:肩、手、小腿具有支撐力的護甲，能抵擋近戰傷害。
 韌甲:具有支撐力的護甲，能降低1點弓箭傷害。</t>
   </si>
   <si>
-    <t xml:space="preserve">鎖喉</t>
-  </si>
-  <si>
-    <t xml:space="preserve">念力控場攻擊</t>
+    <t>鎖喉</t>
+  </si>
+  <si>
+    <t>念力控場攻擊</t>
   </si>
   <si>
     <r>
@@ -954,20 +959,20 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">附魔抗性</t>
-  </si>
-  <si>
-    <t xml:space="preserve">提高防禦能力</t>
-  </si>
-  <si>
-    <t xml:space="preserve">提高1點生命，並使承受魔法傷害-1。
+    <t>附魔抗性</t>
+  </si>
+  <si>
+    <t>提高防禦能力</t>
+  </si>
+  <si>
+    <t>提高1點生命，並使承受魔法傷害-1。
 但法力減少1點。</t>
   </si>
   <si>
-    <t xml:space="preserve">致盲</t>
-  </si>
-  <si>
-    <t xml:space="preserve">控場額外傷害</t>
+    <t>致盲</t>
+  </si>
+  <si>
+    <t>控場額外傷害</t>
   </si>
   <si>
     <r>
@@ -998,40 +1003,24 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>可用陣營(BI/AD/JD/DN/NT/ALL)</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="136"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1091,7 +1080,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1099,134 +1088,396 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:L1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="59.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.58"/>
+    <col min="1" max="1" width="8.625" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="60.25" customWidth="1"/>
+    <col min="4" max="4" width="54.375" customWidth="1"/>
+    <col min="5" max="5" width="59.375" customWidth="1"/>
+    <col min="6" max="1025" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -1247,8 +1498,11 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="128.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M1" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="205.5">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1267,11 +1521,14 @@
       <c r="K2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="75">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -1290,11 +1547,14 @@
       <c r="K3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="75">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -1307,17 +1567,20 @@
       <c r="D4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="56.25">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -1336,11 +1599,14 @@
       <c r="K5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
@@ -1353,7 +1619,7 @@
       <c r="D6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -1362,11 +1628,14 @@
       <c r="K6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="75">
       <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
@@ -1382,17 +1651,20 @@
       <c r="E7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7">
         <v>3</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="118.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="168.75">
       <c r="A8" s="4" t="s">
         <v>38</v>
       </c>
@@ -1411,11 +1683,14 @@
       <c r="K8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -1437,11 +1712,14 @@
       <c r="K9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="106.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="150">
       <c r="A10" s="4" t="s">
         <v>46</v>
       </c>
@@ -1463,11 +1741,14 @@
       <c r="K10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="91.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="131.25">
       <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
@@ -1489,11 +1770,14 @@
       <c r="K11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="103.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="150">
       <c r="A12" s="4" t="s">
         <v>54</v>
       </c>
@@ -1512,11 +1796,14 @@
       <c r="K12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="121.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="153">
       <c r="A13" s="4" t="s">
         <v>58</v>
       </c>
@@ -1535,11 +1822,14 @@
       <c r="K13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="173.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="281.25">
       <c r="A14" s="4" t="s">
         <v>62</v>
       </c>
@@ -1561,11 +1851,14 @@
       <c r="K14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="4" t="s">
         <v>66</v>
       </c>
@@ -1581,17 +1874,20 @@
       <c r="E15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15">
         <v>-3</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="28.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="37.5">
       <c r="A16" s="4" t="s">
         <v>71</v>
       </c>
@@ -1616,11 +1912,14 @@
       <c r="K16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="L16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="83.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="112.5">
       <c r="A17" s="4" t="s">
         <v>76</v>
       </c>
@@ -1639,11 +1938,14 @@
       <c r="K17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="L17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="4" t="s">
         <v>79</v>
       </c>
@@ -1668,11 +1970,14 @@
       <c r="K18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="0" t="n">
+      <c r="L18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="4" t="s">
         <v>81</v>
       </c>
@@ -1697,11 +2002,14 @@
       <c r="K19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L19" s="0" t="n">
+      <c r="L19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="65.25">
       <c r="A20" s="4" t="s">
         <v>84</v>
       </c>
@@ -1720,17 +2028,20 @@
       <c r="F20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20">
         <v>6</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L20" s="0" t="n">
+      <c r="L20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="95.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="118.5">
       <c r="A21" s="4" t="s">
         <v>87</v>
       </c>
@@ -1755,11 +2066,14 @@
       <c r="K21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L21" s="0" t="n">
+      <c r="L21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="163.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="225">
       <c r="A22" s="4" t="s">
         <v>89</v>
       </c>
@@ -1778,11 +2092,14 @@
       <c r="K22" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="0" t="n">
+      <c r="L22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="129.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="187.5">
       <c r="A23" s="4" t="s">
         <v>92</v>
       </c>
@@ -1798,17 +2115,20 @@
       <c r="E23" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="9" t="n">
+      <c r="H23" s="9">
         <v>-2</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L23" s="0" t="n">
+      <c r="L23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="129.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="187.5">
       <c r="A24" s="4" t="s">
         <v>95</v>
       </c>
@@ -1827,11 +2147,14 @@
       <c r="K24" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L24" s="0" t="n">
+      <c r="L24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="28.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="37.5">
       <c r="A25" s="4" t="s">
         <v>98</v>
       </c>
@@ -1850,11 +2173,14 @@
       <c r="K25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L25" s="0" t="n">
+      <c r="L25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="118.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="187.5">
       <c r="A26" s="4" t="s">
         <v>101</v>
       </c>
@@ -1873,15 +2199,18 @@
       <c r="K26" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="L26" s="0" t="n">
+      <c r="L26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="91.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="105">
       <c r="A27" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>104</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1893,178 +2222,183 @@
       <c r="E27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="0" t="s">
+      <c r="K27" t="s">
         <v>17</v>
       </c>
-      <c r="L27" s="0" t="n">
+      <c r="L27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="118.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="M27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="206.25">
+      <c r="A28" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" t="s">
         <v>108</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" t="s">
         <v>27</v>
       </c>
-      <c r="K28" s="0" t="s">
+      <c r="K28" t="s">
         <v>17</v>
       </c>
-      <c r="L28" s="0" t="n">
+      <c r="L28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="155.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="M28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="262.5">
+      <c r="A29" t="s">
         <v>110</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" t="s">
         <v>111</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" t="s">
         <v>57</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K29" s="0" t="s">
+      <c r="K29" t="s">
         <v>17</v>
       </c>
-      <c r="L29" s="0" t="n">
+      <c r="L29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="65.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="M29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="93.75">
+      <c r="A30" t="s">
         <v>113</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" t="s">
         <v>114</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" t="s">
         <v>27</v>
       </c>
-      <c r="K30" s="0" t="s">
+      <c r="K30" t="s">
         <v>44</v>
       </c>
-      <c r="L30" s="0" t="n">
+      <c r="L30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="129.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="M30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="225">
+      <c r="A31" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" t="s">
         <v>117</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" t="s">
         <v>57</v>
       </c>
-      <c r="K31" s="0" t="s">
+      <c r="K31" t="s">
         <v>44</v>
       </c>
-      <c r="L31" s="0" t="n">
+      <c r="L31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="31.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="M31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="37.5">
+      <c r="A32" t="s">
         <v>119</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" t="s">
         <v>120</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" t="s">
         <v>57</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H32" s="12" t="n">
+      <c r="H32" s="12">
         <v>-1</v>
       </c>
-      <c r="K32" s="0" t="s">
+      <c r="K32" t="s">
         <v>17</v>
       </c>
-      <c r="L32" s="0" t="n">
+      <c r="L32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="136.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="M32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="206.25">
+      <c r="A33" t="s">
         <v>122</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" t="s">
         <v>123</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" t="s">
         <v>44</v>
       </c>
-      <c r="K33" s="0" t="s">
+      <c r="K33" t="s">
         <v>44</v>
       </c>
-      <c r="L33" s="0" t="n">
+      <c r="L33">
         <v>1</v>
       </c>
-    </row>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="M33" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>